<commit_message>
Adding in species BLAST assignment code
</commit_message>
<xml_diff>
--- a/Raw_data/site_extractions.xlsx
+++ b/Raw_data/site_extractions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsasaki/Desktop/Lab_Projects/diapt_ctmax_survey/Raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01EF3623-F16A-7448-B7C2-3592D0044C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86A18A0-20E9-AD44-927F-8A28D2E78E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{70252E7D-B877-DF4F-9713-FDF3EF035878}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
   <si>
     <t>site</t>
   </si>
@@ -182,24 +182,9 @@
     <t>Canterbury Pond</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Sequences</t>
   </si>
   <si>
-    <t>SM</t>
-  </si>
-  <si>
-    <t>SP</t>
-  </si>
-  <si>
-    <t>SR</t>
-  </si>
-  <si>
-    <t>SO</t>
-  </si>
-  <si>
     <t>Code</t>
   </si>
   <si>
@@ -224,9 +209,6 @@
     <t>PL</t>
   </si>
   <si>
-    <t>OP</t>
-  </si>
-  <si>
     <t>LW</t>
   </si>
   <si>
@@ -258,6 +240,9 @@
   </si>
   <si>
     <t>LC</t>
+  </si>
+  <si>
+    <t>Ow</t>
   </si>
 </sst>
 </file>
@@ -679,7 +664,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -704,10 +689,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="8" customFormat="1">
@@ -792,10 +777,10 @@
         <v>-105.042222</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="F6" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -826,10 +811,10 @@
         <v>-105.819607</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
+      </c>
+      <c r="F8" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="8" customFormat="1">
@@ -897,10 +882,10 @@
         <v>-70.841425999999998</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
+      </c>
+      <c r="F12" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -917,10 +902,10 @@
         <v>-71.368792999999997</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
+      </c>
+      <c r="F13" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="12" customFormat="1">
@@ -954,10 +939,10 @@
         <v>-73.406449199999997</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>48</v>
+        <v>54</v>
+      </c>
+      <c r="F15" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -974,10 +959,10 @@
         <v>-73.290063000000004</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>48</v>
+        <v>55</v>
+      </c>
+      <c r="F16" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="12" customFormat="1">
@@ -1011,10 +996,10 @@
         <v>-72.886409</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>48</v>
+        <v>56</v>
+      </c>
+      <c r="F18" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="8" customFormat="1">
@@ -1048,13 +1033,10 @@
         <v>-82.430564000000004</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F20" s="3">
         <v>3</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1071,10 +1053,10 @@
         <v>-77.920331099999999</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>48</v>
+        <v>57</v>
+      </c>
+      <c r="F21" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1091,10 +1073,10 @@
         <v>-79.879589999999993</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>48</v>
+        <v>58</v>
+      </c>
+      <c r="F22" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1111,13 +1093,10 @@
         <v>-77.358057000000002</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F23" s="3">
         <v>3</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1134,10 +1113,10 @@
         <v>-76.882706999999996</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>48</v>
+        <v>60</v>
+      </c>
+      <c r="F24" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1154,13 +1133,10 @@
         <v>-75.731083999999996</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F25" s="3">
         <v>3</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1177,13 +1153,10 @@
         <v>-74.975570000000005</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F26" s="3">
         <v>2</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1200,10 +1173,10 @@
         <v>-83.022433000000007</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>48</v>
+        <v>63</v>
+      </c>
+      <c r="F27" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1220,10 +1193,10 @@
         <v>-80.538070000000005</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>48</v>
+        <v>64</v>
+      </c>
+      <c r="F28" s="3">
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1240,10 +1213,10 @@
         <v>-80.138642000000004</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>48</v>
+        <v>65</v>
+      </c>
+      <c r="F29" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1260,10 +1233,10 @@
         <v>-78.561786999999995</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>48</v>
+        <v>66</v>
+      </c>
+      <c r="F30" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1308,10 +1281,10 @@
         <v>-73.225581000000005</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>48</v>
+        <v>67</v>
+      </c>
+      <c r="F33" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:6">

</xml_diff>

<commit_message>
Adding csv version of site data
</commit_message>
<xml_diff>
--- a/Raw_data/site_extractions.xlsx
+++ b/Raw_data/site_extractions.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsasaki/Desktop/Lab_Projects/diapt_ctmax_survey/Raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A28455-28E1-304B-8B2C-696AD65FB36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C914608E-C9F7-FE4D-9980-7D02B0AA6447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{70252E7D-B877-DF4F-9713-FDF3EF035878}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{70252E7D-B877-DF4F-9713-FDF3EF035878}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="81">
   <si>
     <t>site</t>
   </si>
@@ -267,6 +267,18 @@
   </si>
   <si>
     <t>SL</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Meduxnekeag Lake</t>
+  </si>
+  <si>
+    <t>Fraser</t>
+  </si>
+  <si>
+    <t>Pontoosuc Lake</t>
   </si>
 </sst>
 </file>
@@ -677,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{681DA912-16C1-0D41-B94E-A4D9A4706D3F}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -758,121 +770,109 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5"/>
+        <v>78</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="1">
-        <v>4</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" s="1" customFormat="1">
       <c r="A8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>8</v>
+        <v>35</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="1">
         <v>4</v>
@@ -880,27 +880,21 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="1">
-        <v>3</v>
-      </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E16" s="1">
         <v>4</v>
@@ -908,35 +902,32 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="C17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="1" customFormat="1">
       <c r="A18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="1">
-        <v>3</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="1">
         <v>4</v>
@@ -944,27 +935,21 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="E21" s="1">
         <v>3</v>
@@ -972,13 +957,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E22" s="1">
         <v>4</v>
@@ -986,41 +971,41 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E23" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E24" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E25" s="1">
         <v>4</v>
@@ -1028,41 +1013,41 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E26" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E27" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E28" s="1">
         <v>4</v>
@@ -1070,44 +1055,95 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E29" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
+      </c>
+      <c r="E31" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E32" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="D37" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" s="1">
+        <f>SUM(E2:E35)</f>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to figures and report format
</commit_message>
<xml_diff>
--- a/Raw_data/site_extractions.xlsx
+++ b/Raw_data/site_extractions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsasaki/Desktop/Lab_Projects/diapt_ctmax_survey/Raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89325777-2867-514F-AD52-31C430F08CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F2FF39-288C-C24A-A413-B6AC97E8BD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{70252E7D-B877-DF4F-9713-FDF3EF035878}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="80">
   <si>
     <t>site</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>Pontoosuc Lake</t>
+  </si>
+  <si>
+    <t>WP</t>
   </si>
 </sst>
 </file>
@@ -686,7 +689,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -762,6 +765,9 @@
       <c r="A5" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
@@ -796,6 +802,9 @@
       <c r="A8" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
@@ -818,6 +827,9 @@
       <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="C10" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="D10" s="2" t="s">
         <v>68</v>
       </c>
@@ -908,6 +920,9 @@
     <row r="18" spans="1:5" s="1" customFormat="1">
       <c r="A18" s="1" t="s">
         <v>78</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5">

</xml_diff>

<commit_message>
Updates to site list CSV
</commit_message>
<xml_diff>
--- a/Raw_data/site_extractions.xlsx
+++ b/Raw_data/site_extractions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsasaki/Desktop/Lab_Projects/diapt_ctmax_survey/Raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F2FF39-288C-C24A-A413-B6AC97E8BD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BE5AFB-6993-8C46-9C62-FDB753214E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{70252E7D-B877-DF4F-9713-FDF3EF035878}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{70252E7D-B877-DF4F-9713-FDF3EF035878}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="82">
   <si>
     <t>site</t>
   </si>
@@ -86,15 +86,9 @@
     <t>Lake Whalom</t>
   </si>
   <si>
-    <t>Horn Pond</t>
-  </si>
-  <si>
     <t>Center Springs Pond</t>
   </si>
   <si>
-    <t>West Thompson Reservoir</t>
-  </si>
-  <si>
     <t>Lake Wilson</t>
   </si>
   <si>
@@ -212,9 +206,6 @@
     <t>OP</t>
   </si>
   <si>
-    <t>Ow</t>
-  </si>
-  <si>
     <t>MH</t>
   </si>
   <si>
@@ -236,18 +227,9 @@
     <t>Nebraska</t>
   </si>
   <si>
-    <t>MB</t>
-  </si>
-  <si>
     <t>MI</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Prep</t>
-  </si>
-  <si>
     <t>Chute River</t>
   </si>
   <si>
@@ -276,6 +258,30 @@
   </si>
   <si>
     <t>WP</t>
+  </si>
+  <si>
+    <t>WH</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>OW</t>
+  </si>
+  <si>
+    <t>Lake Erie</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>LM</t>
+  </si>
+  <si>
+    <t>Columbus</t>
   </si>
 </sst>
 </file>
@@ -306,12 +312,18 @@
       <name val="ArialMT"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -335,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -350,6 +362,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -686,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{681DA912-16C1-0D41-B94E-A4D9A4706D3F}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -701,7 +720,7 @@
     <col min="6" max="6" width="10.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -709,44 +728,37 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>37</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>58</v>
+      </c>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>65</v>
+      </c>
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -754,401 +766,403 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4"/>
-    </row>
-    <row r="5" spans="1:5" s="1" customFormat="1">
+        <v>56</v>
+      </c>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E6"/>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="1" customFormat="1">
+        <v>38</v>
+      </c>
+      <c r="D7" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1">
       <c r="A8" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>39</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>73</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="C11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>41</v>
+      </c>
+      <c r="D13" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="D16" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="1" customFormat="1">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="1" customFormat="1">
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="C18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="1">
+      <c r="D21" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="D22" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="D23" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="1">
+      <c r="D24" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="D25" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E26" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="1" t="s">
+      <c r="C28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E27" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E28" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E29" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="D29" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E30" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="D30" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E31" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>79</v>
+      </c>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E32" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>80</v>
+      </c>
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>65</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="1:4">
       <c r="C35" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="D37" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E37" s="1">
-        <f>SUM(E2:E35)</f>
+        <v>69</v>
+      </c>
+      <c r="D35" s="1">
+        <f>SUM(D2:D33)</f>
         <v>74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final batch of sequences
</commit_message>
<xml_diff>
--- a/Raw_data/site_extractions.xlsx
+++ b/Raw_data/site_extractions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewsasaki/Desktop/Lab_Projects/diapt_ctmax_survey/Raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BE5AFB-6993-8C46-9C62-FDB753214E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA881A7-A392-CC48-9C57-04CB9EC3315E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{70252E7D-B877-DF4F-9713-FDF3EF035878}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
   <si>
     <t>site</t>
   </si>
@@ -200,9 +200,6 @@
     <t>BR</t>
   </si>
   <si>
-    <t>CL</t>
-  </si>
-  <si>
     <t>OP</t>
   </si>
   <si>
@@ -275,13 +272,19 @@
     <t>Lake Erie</t>
   </si>
   <si>
+    <t>LM</t>
+  </si>
+  <si>
+    <t>Columbus</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
     <t>ER</t>
-  </si>
-  <si>
-    <t>LM</t>
-  </si>
-  <si>
-    <t>Columbus</t>
   </si>
 </sst>
 </file>
@@ -708,7 +711,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -736,25 +739,25 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" s="6"/>
     </row>
@@ -766,13 +769,13 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1">
       <c r="A5" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -780,13 +783,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="D6" s="7"/>
     </row>
@@ -806,13 +809,13 @@
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1">
       <c r="A8" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" s="6"/>
     </row>
@@ -838,7 +841,7 @@
         <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" s="6"/>
     </row>
@@ -850,7 +853,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D11" s="6"/>
     </row>
@@ -890,7 +893,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" s="6"/>
     </row>
@@ -924,7 +927,7 @@
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1">
       <c r="A17" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
@@ -952,7 +955,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D19" s="6">
         <v>3</v>
@@ -1050,7 +1053,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D26" s="1">
         <v>4</v>
@@ -1106,7 +1109,7 @@
         <v>11</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="D30" s="1">
         <v>4</v>
@@ -1114,52 +1117,52 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D31" s="6"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D32" s="6"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="D33" s="6"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="D34" s="8"/>
     </row>
     <row r="35" spans="1:4">
       <c r="C35" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D35" s="1">
         <f>SUM(D2:D33)</f>

</xml_diff>